<commit_message>
Reorganization of data folders
</commit_message>
<xml_diff>
--- a/data/reports/player_0_analysis.xlsx
+++ b/data/reports/player_0_analysis.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="240">
   <si>
     <t>Player 0 Analytics</t>
   </si>
@@ -30,7 +30,7 @@
     <t>Video ID:</t>
   </si>
   <si>
-    <t>t2omui24nswm</t>
+    <t>rgz7fo9wohv4</t>
   </si>
   <si>
     <t>PERFORMANCE GRADES</t>
@@ -39,7 +39,7 @@
     <t>Serve Depth Grade</t>
   </si>
   <si>
-    <t>Intermediate</t>
+    <t>Advanced</t>
   </si>
   <si>
     <t>Serve Height Grade</t>
@@ -165,15 +165,15 @@
     <t>Returning</t>
   </si>
   <si>
+    <t>40.0%</t>
+  </si>
+  <si>
+    <t>Serving</t>
+  </si>
+  <si>
     <t>0.0%</t>
   </si>
   <si>
-    <t>Serving</t>
-  </si>
-  <si>
-    <t>33.3%</t>
-  </si>
-  <si>
     <t>SUMMARY</t>
   </si>
   <si>
@@ -195,7 +195,16 @@
     <t>Quality Score</t>
   </si>
   <si>
-    <t xml:space="preserve">Rally 23, Shot </t>
+    <t xml:space="preserve">Rally 0, Shot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rally 10, Shot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rally 17, Shot </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rally 18, Shot </t>
   </si>
   <si>
     <t>Rally</t>
@@ -222,682 +231,514 @@
     <t>Height (ft)</t>
   </si>
   <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>serve</t>
+  </si>
+  <si>
+    <t>19833</t>
+  </si>
+  <si>
+    <t>20733</t>
+  </si>
+  <si>
+    <t>46.048</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>drive</t>
+  </si>
+  <si>
+    <t>rally</t>
+  </si>
+  <si>
+    <t>22733</t>
+  </si>
+  <si>
+    <t>23733</t>
+  </si>
+  <si>
+    <t>39.679</t>
+  </si>
+  <si>
+    <t>3.89</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>drop</t>
+  </si>
+  <si>
+    <t>25566</t>
+  </si>
+  <si>
+    <t>26733</t>
+  </si>
+  <si>
+    <t>31.607</t>
+  </si>
+  <si>
+    <t>4.558</t>
+  </si>
+  <si>
     <t>1</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>serve</t>
-  </si>
-  <si>
-    <t>16583</t>
-  </si>
-  <si>
-    <t>17751</t>
-  </si>
-  <si>
-    <t>45.348</t>
-  </si>
-  <si>
-    <t>5.636</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>drop</t>
-  </si>
-  <si>
-    <t>rally</t>
-  </si>
-  <si>
-    <t>19252</t>
-  </si>
-  <si>
-    <t>20153</t>
-  </si>
-  <si>
-    <t>34.035</t>
-  </si>
-  <si>
-    <t>3.302</t>
-  </si>
-  <si>
     <t>return</t>
   </si>
   <si>
-    <t>32232</t>
-  </si>
-  <si>
-    <t>33266</t>
-  </si>
-  <si>
-    <t>32.444</t>
-  </si>
-  <si>
-    <t>3.545</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>drive</t>
-  </si>
-  <si>
-    <t>35135</t>
-  </si>
-  <si>
-    <t>36136</t>
-  </si>
-  <si>
-    <t>41.915</t>
-  </si>
-  <si>
-    <t>3.906</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>54921</t>
-  </si>
-  <si>
-    <t>55955</t>
-  </si>
-  <si>
-    <t>38.949</t>
-  </si>
-  <si>
-    <t>3.09</t>
+    <t>41900</t>
+  </si>
+  <si>
+    <t>42800</t>
+  </si>
+  <si>
+    <t>31.255</t>
+  </si>
+  <si>
+    <t>44366</t>
+  </si>
+  <si>
+    <t>45266</t>
+  </si>
+  <si>
+    <t>19.61</t>
+  </si>
+  <si>
+    <t>5.88</t>
+  </si>
+  <si>
+    <t>55733</t>
+  </si>
+  <si>
+    <t>57033</t>
+  </si>
+  <si>
+    <t>37.044</t>
+  </si>
+  <si>
+    <t>6.464</t>
+  </si>
+  <si>
+    <t>70366</t>
+  </si>
+  <si>
+    <t>71400</t>
+  </si>
+  <si>
+    <t>38.631</t>
+  </si>
+  <si>
+    <t>3.169</t>
+  </si>
+  <si>
+    <t>smash</t>
+  </si>
+  <si>
+    <t>72900</t>
+  </si>
+  <si>
+    <t>73233</t>
+  </si>
+  <si>
+    <t>22.366</t>
+  </si>
+  <si>
+    <t>3.223</t>
+  </si>
+  <si>
+    <t>87666</t>
+  </si>
+  <si>
+    <t>88633</t>
+  </si>
+  <si>
+    <t>41.877</t>
+  </si>
+  <si>
+    <t>3.012</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>111066</t>
+  </si>
+  <si>
+    <t>112266</t>
+  </si>
+  <si>
+    <t>40.088</t>
+  </si>
+  <si>
+    <t>4.806</t>
+  </si>
+  <si>
+    <t>114433</t>
+  </si>
+  <si>
+    <t>115800</t>
+  </si>
+  <si>
+    <t>36.104</t>
+  </si>
+  <si>
+    <t>5.179</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>77143</t>
-  </si>
-  <si>
-    <t>78278</t>
-  </si>
-  <si>
-    <t>47.71</t>
-  </si>
-  <si>
-    <t>5.659</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>87620</t>
-  </si>
-  <si>
-    <t>88755</t>
-  </si>
-  <si>
-    <t>43.149</t>
-  </si>
-  <si>
-    <t>3.696</t>
+    <t>117833</t>
+  </si>
+  <si>
+    <t>118433</t>
+  </si>
+  <si>
+    <t>16.418</t>
+  </si>
+  <si>
+    <t>3.34</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>97263</t>
-  </si>
-  <si>
-    <t>98331</t>
-  </si>
-  <si>
-    <t>42.981</t>
-  </si>
-  <si>
-    <t>3.908</t>
-  </si>
-  <si>
-    <t>100166</t>
-  </si>
-  <si>
-    <t>100934</t>
-  </si>
-  <si>
-    <t>28.256</t>
+    <t>133400</t>
+  </si>
+  <si>
+    <t>134533</t>
+  </si>
+  <si>
+    <t>38.347</t>
+  </si>
+  <si>
+    <t>4.525</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>112112</t>
-  </si>
-  <si>
-    <t>113013</t>
-  </si>
-  <si>
-    <t>35.238</t>
+    <t>146966</t>
+  </si>
+  <si>
+    <t>148300</t>
+  </si>
+  <si>
+    <t>45.596</t>
+  </si>
+  <si>
+    <t>7.132</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>156800</t>
+  </si>
+  <si>
+    <t>157833</t>
+  </si>
+  <si>
+    <t>34.901</t>
+  </si>
+  <si>
+    <t>4.575</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
-    <t>137437</t>
-  </si>
-  <si>
-    <t>138238</t>
-  </si>
-  <si>
-    <t>39.046</t>
+    <t>173966</t>
+  </si>
+  <si>
+    <t>174800</t>
+  </si>
+  <si>
+    <t>40.87</t>
+  </si>
+  <si>
+    <t>176766</t>
+  </si>
+  <si>
+    <t>178266</t>
+  </si>
+  <si>
+    <t>41.056</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>149049</t>
-  </si>
-  <si>
-    <t>149949</t>
-  </si>
-  <si>
-    <t>38.76</t>
+    <t>190666</t>
+  </si>
+  <si>
+    <t>192266</t>
+  </si>
+  <si>
+    <t>46.47</t>
+  </si>
+  <si>
+    <t>5.251</t>
   </si>
   <si>
     <t>12</t>
   </si>
   <si>
-    <t>159392</t>
-  </si>
-  <si>
-    <t>160393</t>
-  </si>
-  <si>
-    <t>39.147</t>
-  </si>
-  <si>
-    <t>3.364</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>176810</t>
-  </si>
-  <si>
-    <t>177877</t>
-  </si>
-  <si>
-    <t>40.384</t>
-  </si>
-  <si>
-    <t>4.577</t>
-  </si>
-  <si>
-    <t>179546</t>
-  </si>
-  <si>
-    <t>180580</t>
-  </si>
-  <si>
-    <t>38.435</t>
+    <t>203500</t>
+  </si>
+  <si>
+    <t>203733</t>
+  </si>
+  <si>
+    <t>19.461</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>227366</t>
+  </si>
+  <si>
+    <t>228266</t>
+  </si>
+  <si>
+    <t>37.406</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>236500</t>
+  </si>
+  <si>
+    <t>237333</t>
+  </si>
+  <si>
+    <t>42.009</t>
+  </si>
+  <si>
+    <t>239133</t>
+  </si>
+  <si>
+    <t>239866</t>
+  </si>
+  <si>
+    <t>26.282</t>
   </si>
   <si>
     <t>16</t>
   </si>
   <si>
-    <t>230430</t>
-  </si>
-  <si>
-    <t>231664</t>
-  </si>
-  <si>
-    <t>42.029</t>
-  </si>
-  <si>
-    <t>5.201</t>
-  </si>
-  <si>
-    <t>233400</t>
-  </si>
-  <si>
-    <t>234267</t>
-  </si>
-  <si>
-    <t>39.299</t>
+    <t>252666</t>
+  </si>
+  <si>
+    <t>253866</t>
+  </si>
+  <si>
+    <t>32.308</t>
+  </si>
+  <si>
+    <t>4.649</t>
   </si>
   <si>
     <t>17</t>
   </si>
   <si>
-    <t>246813</t>
-  </si>
-  <si>
-    <t>247847</t>
-  </si>
-  <si>
-    <t>39.138</t>
-  </si>
-  <si>
-    <t>4.479</t>
-  </si>
-  <si>
-    <t>249482</t>
-  </si>
-  <si>
-    <t>249783</t>
-  </si>
-  <si>
-    <t>22.27</t>
+    <t>271366</t>
+  </si>
+  <si>
+    <t>272300</t>
+  </si>
+  <si>
+    <t>41.071</t>
+  </si>
+  <si>
+    <t>3.518</t>
+  </si>
+  <si>
+    <t>274933</t>
+  </si>
+  <si>
+    <t>275766</t>
+  </si>
+  <si>
+    <t>34.099</t>
+  </si>
+  <si>
+    <t>3.143</t>
+  </si>
+  <si>
+    <t>278133</t>
+  </si>
+  <si>
+    <t>279400</t>
+  </si>
+  <si>
+    <t>30.724</t>
+  </si>
+  <si>
+    <t>4.638</t>
   </si>
   <si>
     <t>18</t>
   </si>
   <si>
-    <t>261861</t>
-  </si>
-  <si>
-    <t>262696</t>
-  </si>
-  <si>
-    <t>30.385</t>
-  </si>
-  <si>
-    <t>264698</t>
-  </si>
-  <si>
-    <t>265532</t>
-  </si>
-  <si>
-    <t>32.424</t>
-  </si>
-  <si>
-    <t>3.259</t>
-  </si>
-  <si>
-    <t>267000</t>
-  </si>
-  <si>
-    <t>268001</t>
-  </si>
-  <si>
-    <t>30.149</t>
-  </si>
-  <si>
-    <t>6.719</t>
-  </si>
-  <si>
-    <t>lob</t>
-  </si>
-  <si>
-    <t>269602</t>
-  </si>
-  <si>
-    <t>271404</t>
-  </si>
-  <si>
-    <t>46.692</t>
-  </si>
-  <si>
-    <t>12.153</t>
+    <t>289666</t>
+  </si>
+  <si>
+    <t>290633</t>
+  </si>
+  <si>
+    <t>44.267</t>
+  </si>
+  <si>
+    <t>292100</t>
+  </si>
+  <si>
+    <t>292966</t>
+  </si>
+  <si>
+    <t>33.449</t>
   </si>
   <si>
     <t>19</t>
   </si>
   <si>
-    <t>302435</t>
-  </si>
-  <si>
-    <t>303503</t>
-  </si>
-  <si>
-    <t>41.407</t>
-  </si>
-  <si>
-    <t>3.447</t>
+    <t>307433</t>
+  </si>
+  <si>
+    <t>308733</t>
+  </si>
+  <si>
+    <t>48.231</t>
+  </si>
+  <si>
+    <t>6.292</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>321700</t>
+  </si>
+  <si>
+    <t>323200</t>
+  </si>
+  <si>
+    <t>40.802</t>
+  </si>
+  <si>
+    <t>8.842</t>
+  </si>
+  <si>
+    <t>325233</t>
+  </si>
+  <si>
+    <t>326433</t>
+  </si>
+  <si>
+    <t>33.986</t>
+  </si>
+  <si>
+    <t>4.504</t>
   </si>
   <si>
     <t>21</t>
   </si>
   <si>
-    <t>332198</t>
-  </si>
-  <si>
-    <t>333166</t>
-  </si>
-  <si>
-    <t>31.703</t>
+    <t>336866</t>
+  </si>
+  <si>
+    <t>338000</t>
+  </si>
+  <si>
+    <t>43.461</t>
+  </si>
+  <si>
+    <t>4.56</t>
   </si>
   <si>
     <t>22</t>
   </si>
   <si>
-    <t>351651</t>
-  </si>
-  <si>
-    <t>352619</t>
-  </si>
-  <si>
-    <t>41.353</t>
-  </si>
-  <si>
-    <t>3.916</t>
-  </si>
-  <si>
-    <t>354387</t>
-  </si>
-  <si>
-    <t>355221</t>
-  </si>
-  <si>
-    <t>35.693</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>375809</t>
-  </si>
-  <si>
-    <t>376676</t>
-  </si>
-  <si>
-    <t>36.755</t>
-  </si>
-  <si>
-    <t>378244</t>
-  </si>
-  <si>
-    <t>379212</t>
-  </si>
-  <si>
-    <t>37.294</t>
-  </si>
-  <si>
-    <t>381147</t>
-  </si>
-  <si>
-    <t>382048</t>
-  </si>
-  <si>
-    <t>36.418</t>
-  </si>
-  <si>
-    <t>24</t>
-  </si>
-  <si>
-    <t>391958</t>
-  </si>
-  <si>
-    <t>392525</t>
-  </si>
-  <si>
-    <t>25.14</t>
+    <t>348133</t>
+  </si>
+  <si>
+    <t>349066</t>
+  </si>
+  <si>
+    <t>38.904</t>
+  </si>
+  <si>
+    <t>3.564</t>
   </si>
   <si>
     <t>25</t>
   </si>
   <si>
-    <t>404604</t>
-  </si>
-  <si>
-    <t>405605</t>
-  </si>
-  <si>
-    <t>33.839</t>
-  </si>
-  <si>
-    <t>3.056</t>
-  </si>
-  <si>
-    <t>407741</t>
-  </si>
-  <si>
-    <t>408541</t>
-  </si>
-  <si>
-    <t>31.743</t>
-  </si>
-  <si>
-    <t>3.72</t>
+    <t>382466</t>
+  </si>
+  <si>
+    <t>382733</t>
+  </si>
+  <si>
+    <t>24.345</t>
   </si>
   <si>
     <t>26</t>
   </si>
   <si>
-    <t>423223</t>
-  </si>
-  <si>
-    <t>424391</t>
-  </si>
-  <si>
-    <t>35.81</t>
-  </si>
-  <si>
-    <t>4.28</t>
+    <t>392866</t>
+  </si>
+  <si>
+    <t>393900</t>
+  </si>
+  <si>
+    <t>41.9</t>
+  </si>
+  <si>
+    <t>395966</t>
+  </si>
+  <si>
+    <t>396666</t>
+  </si>
+  <si>
+    <t>32.4</t>
+  </si>
+  <si>
+    <t>3.689</t>
+  </si>
+  <si>
+    <t>398100</t>
+  </si>
+  <si>
+    <t>398366</t>
+  </si>
+  <si>
+    <t>11.455</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>436036</t>
-  </si>
-  <si>
-    <t>437170</t>
-  </si>
-  <si>
-    <t>36.381</t>
-  </si>
-  <si>
-    <t>4.187</t>
-  </si>
-  <si>
-    <t>28</t>
-  </si>
-  <si>
-    <t>446279</t>
-  </si>
-  <si>
-    <t>447180</t>
-  </si>
-  <si>
-    <t>40.539</t>
-  </si>
-  <si>
-    <t>3.486</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>460527</t>
-  </si>
-  <si>
-    <t>461528</t>
-  </si>
-  <si>
-    <t>41.089</t>
-  </si>
-  <si>
-    <t>3.809</t>
-  </si>
-  <si>
-    <t>31</t>
-  </si>
-  <si>
-    <t>485852</t>
-  </si>
-  <si>
-    <t>486853</t>
-  </si>
-  <si>
-    <t>40.435</t>
-  </si>
-  <si>
-    <t>3.405</t>
-  </si>
-  <si>
-    <t>488521</t>
-  </si>
-  <si>
-    <t>489989</t>
-  </si>
-  <si>
-    <t>30.668</t>
-  </si>
-  <si>
-    <t>9.338</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>499332</t>
-  </si>
-  <si>
-    <t>500367</t>
-  </si>
-  <si>
-    <t>36.197</t>
-  </si>
-  <si>
-    <t>3.505</t>
-  </si>
-  <si>
-    <t>501968</t>
-  </si>
-  <si>
-    <t>503036</t>
-  </si>
-  <si>
-    <t>35.965</t>
-  </si>
-  <si>
-    <t>4.841</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>517117</t>
-  </si>
-  <si>
-    <t>518284</t>
-  </si>
-  <si>
-    <t>45.599</t>
-  </si>
-  <si>
-    <t>5.31</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>529162</t>
-  </si>
-  <si>
-    <t>530296</t>
-  </si>
-  <si>
-    <t>37.01</t>
-  </si>
-  <si>
-    <t>4.6</t>
-  </si>
-  <si>
-    <t>531898</t>
-  </si>
-  <si>
-    <t>532866</t>
-  </si>
-  <si>
-    <t>35.635</t>
-  </si>
-  <si>
-    <t>3.657</t>
-  </si>
-  <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>541207</t>
-  </si>
-  <si>
-    <t>542208</t>
-  </si>
-  <si>
-    <t>43.424</t>
-  </si>
-  <si>
-    <t>5.115</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>549149</t>
-  </si>
-  <si>
-    <t>550183</t>
-  </si>
-  <si>
-    <t>39.892</t>
-  </si>
-  <si>
-    <t>4.363</t>
-  </si>
-  <si>
-    <t>551885</t>
-  </si>
-  <si>
-    <t>552585</t>
-  </si>
-  <si>
-    <t>26.265</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>566499</t>
-  </si>
-  <si>
-    <t>567867</t>
-  </si>
-  <si>
-    <t>42.958</t>
-  </si>
-  <si>
-    <t>6.558</t>
-  </si>
-  <si>
-    <t>570503</t>
-  </si>
-  <si>
-    <t>571471</t>
-  </si>
-  <si>
-    <t>34.428</t>
-  </si>
-  <si>
-    <t>4.004</t>
-  </si>
-  <si>
-    <t>38</t>
-  </si>
-  <si>
-    <t>582482</t>
-  </si>
-  <si>
-    <t>583450</t>
-  </si>
-  <si>
-    <t>38.868</t>
-  </si>
-  <si>
-    <t>4.337</t>
+    <t>410366</t>
+  </si>
+  <si>
+    <t>410866</t>
+  </si>
+  <si>
+    <t>19.357</t>
   </si>
 </sst>
 </file>
@@ -977,7 +818,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF59E0B"/>
+        <fgColor rgb="FF10B981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1422,7 +1263,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="3">
-        <v>4.219849999999999</v>
+        <v>3.80381818181818</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1430,7 +1271,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3">
-        <v>3.925842105263158</v>
+        <v>3.2654</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1438,7 +1279,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3">
-        <v>33.33333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1446,7 +1287,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3">
-        <v>6.707999999999999</v>
+        <v>7.654538461538465</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1454,7 +1295,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="3">
-        <v>4.1615</v>
+        <v>5.336818181818182</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1462,7 +1303,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1470,7 +1311,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="3">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1478,7 +1319,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1543,7 +1384,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="3">
-        <v>39.78015</v>
+        <v>40.19618181818182</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1551,7 +1392,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="3">
-        <v>3.925842105263158</v>
+        <v>3.2654</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1559,7 +1400,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="3">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1591,7 +1432,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="3">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1615,7 +1456,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="3">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1623,7 +1464,7 @@
         <v>40</v>
       </c>
       <c r="B17" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1654,7 +1495,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="3">
-        <v>37.292</v>
+        <v>36.34546153846154</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1662,7 +1503,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="3">
-        <v>4.161500000000001</v>
+        <v>5.336818181818182</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1670,7 +1511,7 @@
         <v>42</v>
       </c>
       <c r="B6" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1702,7 +1543,7 @@
         <v>36</v>
       </c>
       <c r="B11" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1726,7 +1567,7 @@
         <v>39</v>
       </c>
       <c r="B16" s="3">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1734,7 +1575,7 @@
         <v>40</v>
       </c>
       <c r="B17" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1796,7 +1637,7 @@
         <v>52</v>
       </c>
       <c r="B10" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1804,7 +1645,7 @@
         <v>53</v>
       </c>
       <c r="B11" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1812,7 +1653,7 @@
         <v>54</v>
       </c>
       <c r="B12" s="3">
-        <v>8.333333333333332</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1822,7 +1663,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1852,6 +1693,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1859,7 +1727,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1870,172 +1738,172 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>99</v>
@@ -2052,80 +1920,80 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2133,13 +2001,13 @@
         <v>116</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>117</v>
@@ -2151,21 +2019,21 @@
         <v>119</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>121</v>
@@ -2177,1016 +2045,700 @@
         <v>123</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>87</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="3" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>68</v>
+        <v>125</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>87</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>145</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="3" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="3" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>168</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="H23" s="3"/>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" s="3" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>169</v>
+        <v>71</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>87</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" s="3" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>87</v>
+        <v>201</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>87</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="H32" s="3"/>
+        <v>209</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>218</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="H35" s="3"/>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>223</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" s="3" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>233</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="H38" s="3"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>284</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>289</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>292</v>
-      </c>
+      <c r="H39" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>